<commit_message>
Regenerated SML output after merge
</commit_message>
<xml_diff>
--- a/output/SharedMedicinesList/composition-sml-1.xlsx
+++ b/output/SharedMedicinesList/composition-sml-1.xlsx
@@ -206,7 +206,7 @@
     <t>Resource.meta</t>
   </si>
   <si>
-    <t xml:space="preserve">inv-dh-cmp-01:One meta.profile shall be 'http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/composition-sml-1' {Composition.meta.profile.where($this='http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/composition-sml-1').exists()}
+    <t xml:space="preserve">inv-dh-cmp-01:One meta.profile shall be 'http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/composition-sml-1' {profile.where($this='http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/composition-sml-1').exists()}
 </t>
   </si>
   <si>
@@ -514,7 +514,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() | (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}inv-dh-cmp-06:A practitioner shall conform to Base Practitioner {Composition.extension('http://hl7.org.au/fhir/StructureDefinition/information-recipient').resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitioner-dh-base-1')}inv-dh-cmp-07:A patient shall conform to Base Patient {Composition.extension('http://hl7.org.au/fhir/StructureDefinition/information-recipient').resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-dh-base-1')}inv-dh-cmp-08:A related person shall conform to Base RelatedPerson {Composition.extension('http://hl7.org.au/fhir/StructureDefinition/information-recipient').resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/relatedperson-dh-base-1')}inv-dh-cmp-09:A practitioner role shall conform to Base PractitionerRole {Composition.extension('http://hl7.org.au/fhir/StructureDefinition/information-recipient').resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitionerrole-dh-base-1')}inv-dh-cmp-10:An organisation shall conform to Base Organization {Composition.extension('http://hl7.org.au/fhir/StructureDefinition/information-recipient').resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/organization-dh-base-1')}</t>
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}inv-dh-cmp-06:A practitioner shall conform to Base Practitioner {Composition.extension('http://hl7.org.au/fhir/StructureDefinition/information-recipient').resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitioner-dh-base-1')}inv-dh-cmp-07:A patient shall conform to Base Patient {Composition.extension('http://hl7.org.au/fhir/StructureDefinition/information-recipient').resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/patient-dh-base-1')}inv-dh-cmp-08:A related person shall conform to Base RelatedPerson {Composition.extension('http://hl7.org.au/fhir/StructureDefinition/information-recipient').resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/relatedperson-dh-base-1')}inv-dh-cmp-09:A practitioner role shall conform to Base PractitionerRole {Composition.extension('http://hl7.org.au/fhir/StructureDefinition/information-recipient').resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/practitionerrole-dh-base-1')}inv-dh-cmp-10:An organisation shall conform to Base Organization {Composition.extension('http://hl7.org.au/fhir/StructureDefinition/information-recipient').resolve().conformsTo('http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/organization-dh-base-1')}inv-dh-cmp-10:Information recipient shall not be a device {TBD}</t>
   </si>
   <si>
     <t>Composition.modifierExtension</t>
@@ -1392,7 +1392,7 @@
 &lt;/valueCodeableConcept&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/list-meditems-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/observation-norelevantfinding-1)
+    <t xml:space="preserve">Reference(http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/list-meds-current-1|http://ns.electronichealth.net.au/ci/fhir/3.0/StructureDefinition/observation-norelevantfinding-1)
 </t>
   </si>
 </sst>
@@ -4201,7 +4201,7 @@
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="F25" t="s" s="2">
         <v>50</v>

</xml_diff>